<commit_message>
update exploration of remaining depts, and sets manually geoid for each one
</commit_message>
<xml_diff>
--- a/para_comparar.xlsx
+++ b/para_comparar.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/desiertos/side/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F6315188-2EC9-D940-A45B-A99E6485E0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{58FFB29D-156C-6F4B-BE3D-6B8837C6580F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="960" windowWidth="24540" windowHeight="13680" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="960" windowWidth="24540" windowHeight="13680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="para_comparar_dept" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
-    <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
+    <sheet name="comparacao" sheetId="2" r:id="rId2"/>
+    <sheet name="santiago" sheetId="3" r:id="rId3"/>
+    <sheet name="correspondence" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="para_comparar_dept_1" localSheetId="0">para_comparar_dept!$A$1:$B$530</definedName>
-    <definedName name="para_comparar_mun" localSheetId="1">Planilha1!$A$1:$D$55</definedName>
+    <definedName name="para_comparar_mun" localSheetId="1">comparacao!$A$1:$D$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="691">
   <si>
     <t>nam</t>
   </si>
@@ -1422,6 +1423,24 @@
     <t>departamento/municipio/barrio</t>
   </si>
   <si>
+    <t>poblacion_residente</t>
+  </si>
+  <si>
+    <t>cantidad_de_medios</t>
+  </si>
+  <si>
+    <t>cantidad_de_periodistas</t>
+  </si>
+  <si>
+    <t>relacion_poblacion_residente/medios</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>relacion_poblacion_residente/periodistas</t>
+  </si>
+  <si>
     <t>nome_local</t>
   </si>
   <si>
@@ -1452,6 +1471,9 @@
     <t>corpen_aike</t>
   </si>
   <si>
+    <t>santiago_del_estero</t>
+  </si>
+  <si>
     <t>deseado</t>
   </si>
   <si>
@@ -1767,27 +1789,6 @@
     <t>misspelled</t>
   </si>
   <si>
-    <t>DEPARTAMENTO</t>
-  </si>
-  <si>
-    <t>POBLACIÓN RESIDENTE</t>
-  </si>
-  <si>
-    <t>CANTIDAD DE MEDIOS</t>
-  </si>
-  <si>
-    <t>CANTIDAD DE PERIODISTAS</t>
-  </si>
-  <si>
-    <t>RELACIÓN POBLACIÓN RESIDENTE/MEDIOS</t>
-  </si>
-  <si>
-    <t>RELACIÓN POBLACIÓN RESIDENTE/PERIODISTAS</t>
-  </si>
-  <si>
-    <t>CATEGORÍA</t>
-  </si>
-  <si>
     <t>1568.36</t>
   </si>
   <si>
@@ -1888,6 +1889,261 @@
   </si>
   <si>
     <t>procurando os deptos dentro de PBA</t>
+  </si>
+  <si>
+    <t>aguirre</t>
+  </si>
+  <si>
+    <t>alberdi</t>
+  </si>
+  <si>
+    <t>atamisqui</t>
+  </si>
+  <si>
+    <t>avellaneda</t>
+  </si>
+  <si>
+    <t>banda</t>
+  </si>
+  <si>
+    <t>belgrano</t>
+  </si>
+  <si>
+    <t>capital</t>
+  </si>
+  <si>
+    <t>choya</t>
+  </si>
+  <si>
+    <t>copo</t>
+  </si>
+  <si>
+    <t>figueroa</t>
+  </si>
+  <si>
+    <t>loreto</t>
+  </si>
+  <si>
+    <t>mitre</t>
+  </si>
+  <si>
+    <t>moreno</t>
+  </si>
+  <si>
+    <t>pellegrini</t>
+  </si>
+  <si>
+    <t>quebrachos</t>
+  </si>
+  <si>
+    <t>rivadavia</t>
+  </si>
+  <si>
+    <t>robles</t>
+  </si>
+  <si>
+    <t>salavina</t>
+  </si>
+  <si>
+    <t>sarmiento</t>
+  </si>
+  <si>
+    <t>general_taboada</t>
+  </si>
+  <si>
+    <t>guasayan</t>
+  </si>
+  <si>
+    <t>jimenez</t>
+  </si>
+  <si>
+    <t>juan_f_ibarra</t>
+  </si>
+  <si>
+    <t>ojo_de_agua</t>
+  </si>
+  <si>
+    <t>rio_hondo</t>
+  </si>
+  <si>
+    <t>san_martin</t>
+  </si>
+  <si>
+    <t>silipica</t>
+  </si>
+  <si>
+    <t>capital_(posadas)_misiones</t>
+  </si>
+  <si>
+    <t>el_dorado_misiones</t>
+  </si>
+  <si>
+    <t>tolhuin_tierra_del_fuego</t>
+  </si>
+  <si>
+    <t>corpen_aike_santa_cruz</t>
+  </si>
+  <si>
+    <t>deseado_santa_cruz</t>
+  </si>
+  <si>
+    <t>guer_aike_santa_cruz</t>
+  </si>
+  <si>
+    <t>lago_argentino_santa_cruz</t>
+  </si>
+  <si>
+    <t>lago_buenos_aires_santa_cruz</t>
+  </si>
+  <si>
+    <t>magallanes_santa_cruz</t>
+  </si>
+  <si>
+    <t>rio_chico_santa_cruz</t>
+  </si>
+  <si>
+    <t>burrayacu_tucuman</t>
+  </si>
+  <si>
+    <t>juan_bautista_alberdi_tucuman</t>
+  </si>
+  <si>
+    <t>mayor_luis_jorge_fontana_chaco</t>
+  </si>
+  <si>
+    <t>juan_m._de_pueyrredon_san_luis</t>
+  </si>
+  <si>
+    <t>lib._general_san_martin_san_luis</t>
+  </si>
+  <si>
+    <t>loconpue_neuquen</t>
+  </si>
+  <si>
+    <t>corrientes_corrientes</t>
+  </si>
+  <si>
+    <t>adolfo_gonzalez_chaves_buenos_aires</t>
+  </si>
+  <si>
+    <t>carmen_de_patagones_buenos_aires</t>
+  </si>
+  <si>
+    <t>coronel_rosales_buenos_aires</t>
+  </si>
+  <si>
+    <t>general_madariaga_buenos_aires</t>
+  </si>
+  <si>
+    <t>lezama_buenos_aires</t>
+  </si>
+  <si>
+    <t>san_miguel_del_monte_buenos_aires</t>
+  </si>
+  <si>
+    <t>san_nicolas_de_los_arroyos_buenos_aires</t>
+  </si>
+  <si>
+    <t>general_angel_vicente_penaloza_la_rioja</t>
+  </si>
+  <si>
+    <t>general_felipe_varela_la_rioja</t>
+  </si>
+  <si>
+    <t>general_juan_facundo_quiroga_la_rioja</t>
+  </si>
+  <si>
+    <t>general_ortiz_de_ocampo_la_rioja</t>
+  </si>
+  <si>
+    <t>la_rioja_(capital)_la_rioja</t>
+  </si>
+  <si>
+    <t>islas_entre_rios</t>
+  </si>
+  <si>
+    <t>ciudad_de_mendoza_mendoza</t>
+  </si>
+  <si>
+    <t>aguirre_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>alberdi_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>atamisqui_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>avellaneda_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>banda_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>belgrano_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>capital_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>choya_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>copo_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>figueroa_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>general_taboada_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>guasayan_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>jimenez_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>juan_f_ibarra_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>loreto_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>mitre_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>moreno_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>ojo_de_agua_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>pellegrini_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>quebrachos_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>rio_hondo_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>rivadavia_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>robles_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>salavina_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>san_martin_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>sarmiento_santiago_del_estero</t>
+  </si>
+  <si>
+    <t>silipica_santiago_del_estero</t>
   </si>
 </sst>
 </file>
@@ -2472,7 +2728,37 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -7095,8 +7381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E83" sqref="D1:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7113,33 +7399,33 @@
         <v>449</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>448</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="B2" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="C2" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="D2" t="str">
         <f>B2&amp;"_"&amp;C2</f>
@@ -7149,21 +7435,21 @@
         <v>472</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="B3" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="C3" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D55" si="0">B3&amp;"_"&amp;C3</f>
+        <f t="shared" ref="D3:D66" si="0">B3&amp;"_"&amp;C3</f>
         <v>el_dorado_misiones</v>
       </c>
       <c r="E3" s="7">
@@ -7178,7 +7464,7 @@
         <v/>
       </c>
       <c r="H3" s="5" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -7186,10 +7472,10 @@
         <v>217</v>
       </c>
       <c r="B4" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="C4" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -7207,7 +7493,7 @@
         <v>471</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -7215,10 +7501,10 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -7244,10 +7530,10 @@
         <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -7273,10 +7559,10 @@
         <v>369</v>
       </c>
       <c r="B7" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -7302,10 +7588,10 @@
         <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -7331,10 +7617,10 @@
         <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -7360,10 +7646,10 @@
         <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -7389,10 +7675,10 @@
         <v>348</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -7415,13 +7701,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D12" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7442,13 +7728,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D13" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7465,13 +7751,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D14" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7488,13 +7774,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D15" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7511,13 +7797,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>475</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>476</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>468</v>
       </c>
       <c r="D16" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7534,13 +7820,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D17" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7557,13 +7843,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D18" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7580,13 +7866,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D19" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7603,13 +7889,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D20" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7626,13 +7912,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D21" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7649,13 +7935,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D22" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7672,13 +7958,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D23" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7695,13 +7981,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D24" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7718,13 +8004,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D25" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7741,13 +8027,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D26" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7764,13 +8050,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D27" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7787,13 +8073,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D28" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7810,13 +8096,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D29" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7833,13 +8119,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D30" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7856,13 +8142,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D31" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7879,13 +8165,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D32" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7902,13 +8188,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D33" s="9" t="str">
         <f t="shared" si="0"/>
@@ -7925,13 +8211,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="B34" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="C34" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
@@ -7954,10 +8240,10 @@
         <v>286</v>
       </c>
       <c r="B35" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="C35" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
@@ -7978,13 +8264,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="B36" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="C36" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
@@ -8004,13 +8290,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B37" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C37" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -8030,13 +8316,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="B38" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="C38" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -8056,13 +8342,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="B39" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="C39" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -8082,13 +8368,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="B40" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="C40" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -8108,13 +8394,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="B41" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="C41" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
@@ -8134,13 +8420,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="B42" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
       <c r="C42" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
@@ -8160,13 +8446,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
       <c r="B43" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
       <c r="C43" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -8189,13 +8475,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="B44" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="C44" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
@@ -8218,13 +8504,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
       <c r="B45" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="C45" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
@@ -8247,10 +8533,10 @@
         <v>71</v>
       </c>
       <c r="B46" t="s">
+        <v>547</v>
+      </c>
+      <c r="C46" t="s">
         <v>540</v>
-      </c>
-      <c r="C46" t="s">
-        <v>533</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
@@ -8271,13 +8557,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
       <c r="B47" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="C47" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
@@ -8297,13 +8583,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="B48" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="C48" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
@@ -8323,13 +8609,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="B49" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
       <c r="C49" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
@@ -8352,10 +8638,10 @@
         <v>200</v>
       </c>
       <c r="B50" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="C50" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
@@ -8379,10 +8665,10 @@
         <v>246</v>
       </c>
       <c r="B51" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="C51" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
@@ -8406,10 +8692,10 @@
         <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="C52" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
@@ -8430,13 +8716,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="B53" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="C53" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
@@ -8456,13 +8742,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="B54" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="C54" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
@@ -8482,13 +8768,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="B55" t="s">
-        <v>557</v>
+        <v>564</v>
       </c>
       <c r="C55" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
@@ -8510,6 +8796,16 @@
       <c r="A57" t="s">
         <v>167</v>
       </c>
+      <c r="B57" t="s">
+        <v>606</v>
+      </c>
+      <c r="C57" t="s">
+        <v>466</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>aguirre_santiago_del_estero</v>
+      </c>
       <c r="E57">
         <f>G57</f>
         <v>218</v>
@@ -8527,6 +8823,16 @@
       <c r="A58" t="s">
         <v>36</v>
       </c>
+      <c r="B58" t="s">
+        <v>607</v>
+      </c>
+      <c r="C58" t="s">
+        <v>466</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>alberdi_santiago_del_estero</v>
+      </c>
       <c r="E58">
         <f t="shared" ref="E58:E83" si="1">G58</f>
         <v>35</v>
@@ -8544,6 +8850,16 @@
       <c r="A59" t="s">
         <v>276</v>
       </c>
+      <c r="B59" t="s">
+        <v>608</v>
+      </c>
+      <c r="C59" t="s">
+        <v>466</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>atamisqui_santiago_del_estero</v>
+      </c>
       <c r="E59">
         <f t="shared" si="1"/>
         <v>392</v>
@@ -8561,6 +8877,16 @@
       <c r="A60" t="s">
         <v>156</v>
       </c>
+      <c r="B60" t="s">
+        <v>609</v>
+      </c>
+      <c r="C60" t="s">
+        <v>466</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>avellaneda_santiago_del_estero</v>
+      </c>
       <c r="E60" s="5">
         <v>338</v>
       </c>
@@ -8577,6 +8903,16 @@
       <c r="A61" t="s">
         <v>164</v>
       </c>
+      <c r="B61" t="s">
+        <v>610</v>
+      </c>
+      <c r="C61" t="s">
+        <v>466</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>banda_santiago_del_estero</v>
+      </c>
       <c r="E61">
         <f t="shared" si="1"/>
         <v>211</v>
@@ -8594,6 +8930,16 @@
       <c r="A62" t="s">
         <v>141</v>
       </c>
+      <c r="B62" t="s">
+        <v>611</v>
+      </c>
+      <c r="C62" t="s">
+        <v>466</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>belgrano_santiago_del_estero</v>
+      </c>
       <c r="E62" s="5">
         <v>217</v>
       </c>
@@ -8610,6 +8956,16 @@
       <c r="A63" t="s">
         <v>90</v>
       </c>
+      <c r="B63" t="s">
+        <v>612</v>
+      </c>
+      <c r="C63" t="s">
+        <v>466</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>capital_santiago_del_estero</v>
+      </c>
       <c r="E63" s="5">
         <v>244</v>
       </c>
@@ -8626,6 +8982,16 @@
       <c r="A64" t="s">
         <v>45</v>
       </c>
+      <c r="B64" t="s">
+        <v>613</v>
+      </c>
+      <c r="C64" t="s">
+        <v>466</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>choya_santiago_del_estero</v>
+      </c>
       <c r="E64">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -8643,6 +9009,16 @@
       <c r="A65" t="s">
         <v>149</v>
       </c>
+      <c r="B65" t="s">
+        <v>614</v>
+      </c>
+      <c r="C65" t="s">
+        <v>466</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>copo_santiago_del_estero</v>
+      </c>
       <c r="E65">
         <f t="shared" si="1"/>
         <v>181</v>
@@ -8660,6 +9036,16 @@
       <c r="A66" t="s">
         <v>231</v>
       </c>
+      <c r="B66" t="s">
+        <v>615</v>
+      </c>
+      <c r="C66" t="s">
+        <v>466</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v>figueroa_santiago_del_estero</v>
+      </c>
       <c r="E66">
         <f t="shared" si="1"/>
         <v>326</v>
@@ -8677,6 +9063,16 @@
       <c r="A67" t="s">
         <v>38</v>
       </c>
+      <c r="B67" t="s">
+        <v>625</v>
+      </c>
+      <c r="C67" t="s">
+        <v>466</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D84" si="2">B67&amp;"_"&amp;C67</f>
+        <v>general_taboada_santiago_del_estero</v>
+      </c>
       <c r="E67">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -8694,6 +9090,16 @@
       <c r="A68" t="s">
         <v>366</v>
       </c>
+      <c r="B68" t="s">
+        <v>626</v>
+      </c>
+      <c r="C68" t="s">
+        <v>466</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="2"/>
+        <v>guasayan_santiago_del_estero</v>
+      </c>
       <c r="E68">
         <f t="shared" si="1"/>
         <v>220</v>
@@ -8711,6 +9117,16 @@
       <c r="A69" t="s">
         <v>430</v>
       </c>
+      <c r="B69" t="s">
+        <v>627</v>
+      </c>
+      <c r="C69" t="s">
+        <v>466</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="2"/>
+        <v>jimenez_santiago_del_estero</v>
+      </c>
       <c r="E69">
         <f t="shared" si="1"/>
         <v>393</v>
@@ -8728,6 +9144,16 @@
       <c r="A70" t="s">
         <v>589</v>
       </c>
+      <c r="B70" t="s">
+        <v>628</v>
+      </c>
+      <c r="C70" t="s">
+        <v>466</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="2"/>
+        <v>juan_f_ibarra_santiago_del_estero</v>
+      </c>
       <c r="E70" s="7">
         <v>36</v>
       </c>
@@ -8744,6 +9170,16 @@
       <c r="A71" t="s">
         <v>175</v>
       </c>
+      <c r="B71" t="s">
+        <v>616</v>
+      </c>
+      <c r="C71" t="s">
+        <v>466</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="2"/>
+        <v>loreto_santiago_del_estero</v>
+      </c>
       <c r="E71">
         <f t="shared" si="1"/>
         <v>246</v>
@@ -8761,6 +9197,16 @@
       <c r="A72" t="s">
         <v>275</v>
       </c>
+      <c r="B72" t="s">
+        <v>617</v>
+      </c>
+      <c r="C72" t="s">
+        <v>466</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="2"/>
+        <v>mitre_santiago_del_estero</v>
+      </c>
       <c r="E72">
         <f t="shared" si="1"/>
         <v>391</v>
@@ -8778,6 +9224,16 @@
       <c r="A73" t="s">
         <v>24</v>
       </c>
+      <c r="B73" t="s">
+        <v>618</v>
+      </c>
+      <c r="C73" t="s">
+        <v>466</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="2"/>
+        <v>moreno_santiago_del_estero</v>
+      </c>
       <c r="E73" s="5">
         <v>339</v>
       </c>
@@ -8794,6 +9250,16 @@
       <c r="A74" t="s">
         <v>44</v>
       </c>
+      <c r="B74" t="s">
+        <v>629</v>
+      </c>
+      <c r="C74" t="s">
+        <v>466</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="2"/>
+        <v>ojo_de_agua_santiago_del_estero</v>
+      </c>
       <c r="E74">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -8811,6 +9277,16 @@
       <c r="A75" t="s">
         <v>91</v>
       </c>
+      <c r="B75" t="s">
+        <v>619</v>
+      </c>
+      <c r="C75" t="s">
+        <v>466</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="2"/>
+        <v>pellegrini_santiago_del_estero</v>
+      </c>
       <c r="E75" s="5">
         <v>337</v>
       </c>
@@ -8827,6 +9303,16 @@
       <c r="A76" t="s">
         <v>134</v>
       </c>
+      <c r="B76" t="s">
+        <v>620</v>
+      </c>
+      <c r="C76" t="s">
+        <v>466</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="2"/>
+        <v>quebrachos_santiago_del_estero</v>
+      </c>
       <c r="E76">
         <f t="shared" si="1"/>
         <v>154</v>
@@ -8844,6 +9330,16 @@
       <c r="A77" t="s">
         <v>367</v>
       </c>
+      <c r="B77" t="s">
+        <v>630</v>
+      </c>
+      <c r="C77" t="s">
+        <v>466</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="2"/>
+        <v>rio_hondo_santiago_del_estero</v>
+      </c>
       <c r="E77">
         <f t="shared" si="1"/>
         <v>182</v>
@@ -8861,6 +9357,16 @@
       <c r="A78" t="s">
         <v>43</v>
       </c>
+      <c r="B78" t="s">
+        <v>621</v>
+      </c>
+      <c r="C78" t="s">
+        <v>466</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="2"/>
+        <v>rivadavia_santiago_del_estero</v>
+      </c>
       <c r="E78" s="5">
         <v>38</v>
       </c>
@@ -8877,6 +9383,16 @@
       <c r="A79" t="s">
         <v>173</v>
       </c>
+      <c r="B79" t="s">
+        <v>622</v>
+      </c>
+      <c r="C79" t="s">
+        <v>466</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="2"/>
+        <v>robles_santiago_del_estero</v>
+      </c>
       <c r="E79">
         <f t="shared" si="1"/>
         <v>243</v>
@@ -8894,6 +9410,16 @@
       <c r="A80" t="s">
         <v>238</v>
       </c>
+      <c r="B80" t="s">
+        <v>623</v>
+      </c>
+      <c r="C80" t="s">
+        <v>466</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="2"/>
+        <v>salavina_santiago_del_estero</v>
+      </c>
       <c r="E80">
         <f t="shared" si="1"/>
         <v>336</v>
@@ -8911,6 +9437,16 @@
       <c r="A81" t="s">
         <v>355</v>
       </c>
+      <c r="B81" t="s">
+        <v>631</v>
+      </c>
+      <c r="C81" t="s">
+        <v>466</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="2"/>
+        <v>san_martin_santiago_del_estero</v>
+      </c>
       <c r="E81" s="5">
         <v>131</v>
       </c>
@@ -8927,6 +9463,16 @@
       <c r="A82" t="s">
         <v>98</v>
       </c>
+      <c r="B82" t="s">
+        <v>624</v>
+      </c>
+      <c r="C82" t="s">
+        <v>466</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="2"/>
+        <v>sarmiento_santiago_del_estero</v>
+      </c>
       <c r="E82" s="5">
         <v>214</v>
       </c>
@@ -8943,6 +9489,16 @@
       <c r="A83" t="s">
         <v>372</v>
       </c>
+      <c r="B83" t="s">
+        <v>632</v>
+      </c>
+      <c r="C83" t="s">
+        <v>466</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="2"/>
+        <v>silipica_santiago_del_estero</v>
+      </c>
       <c r="E83">
         <f t="shared" si="1"/>
         <v>344</v>
@@ -8957,6 +9513,10 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D84" t="str">
+        <f t="shared" si="2"/>
+        <v>_</v>
+      </c>
       <c r="G84" t="str">
         <f>IF(F84=1,VLOOKUP(A84,para_comparar_dept!$A$2:$B$530,2,FALSE),"")</f>
         <v/>
@@ -8964,22 +9524,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$E$3=$F$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$F4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E55">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$F5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57:E83">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F57=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8989,45 +9549,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>565</v>
+        <v>449</v>
       </c>
       <c r="B1" t="s">
-        <v>566</v>
+        <v>450</v>
       </c>
       <c r="C1" t="s">
-        <v>567</v>
+        <v>451</v>
       </c>
       <c r="D1" t="s">
-        <v>568</v>
+        <v>452</v>
       </c>
       <c r="E1" t="s">
-        <v>569</v>
+        <v>453</v>
       </c>
       <c r="F1" t="s">
-        <v>570</v>
+        <v>455</v>
       </c>
       <c r="G1" t="s">
-        <v>571</v>
+        <v>454</v>
       </c>
       <c r="H1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+      <c r="I1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>167</v>
       </c>
@@ -9046,8 +9615,11 @@
       <c r="H2" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -9072,8 +9644,11 @@
       <c r="H3" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -9098,8 +9673,11 @@
       <c r="H4" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -9124,8 +9702,11 @@
       <c r="H5" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>164</v>
       </c>
@@ -9150,8 +9731,11 @@
       <c r="H6" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -9176,8 +9760,11 @@
       <c r="H7" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -9202,8 +9789,11 @@
       <c r="H8" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -9228,8 +9818,11 @@
       <c r="H9" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -9254,8 +9847,11 @@
       <c r="H10" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>231</v>
       </c>
@@ -9274,8 +9870,11 @@
       <c r="H11" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -9300,8 +9899,11 @@
       <c r="H12" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>366</v>
       </c>
@@ -9320,8 +9922,11 @@
       <c r="H13" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>430</v>
       </c>
@@ -9346,8 +9951,11 @@
       <c r="H14" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>589</v>
       </c>
@@ -9372,8 +9980,11 @@
       <c r="H15" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>175</v>
       </c>
@@ -9398,8 +10009,11 @@
       <c r="H16" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>275</v>
       </c>
@@ -9418,8 +10032,11 @@
       <c r="H17" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -9444,8 +10061,11 @@
       <c r="H18" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -9470,8 +10090,11 @@
       <c r="H19" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -9490,8 +10113,11 @@
       <c r="H20" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>134</v>
       </c>
@@ -9516,8 +10142,11 @@
       <c r="H21" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>367</v>
       </c>
@@ -9542,8 +10171,11 @@
       <c r="H22" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -9568,8 +10200,11 @@
       <c r="H23" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>173</v>
       </c>
@@ -9594,8 +10229,11 @@
       <c r="H24" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>238</v>
       </c>
@@ -9614,8 +10252,11 @@
       <c r="H25" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>355</v>
       </c>
@@ -9634,8 +10275,11 @@
       <c r="H26" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -9660,8 +10304,11 @@
       <c r="H27" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>372</v>
       </c>
@@ -9679,9 +10326,518 @@
       </c>
       <c r="H28" t="s">
         <v>601</v>
+      </c>
+      <c r="I28" t="s">
+        <v>632</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B2" s="5">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B3" s="7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>635</v>
+      </c>
+      <c r="B4">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>637</v>
+      </c>
+      <c r="B6">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>638</v>
+      </c>
+      <c r="B7">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>639</v>
+      </c>
+      <c r="B8">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>640</v>
+      </c>
+      <c r="B9">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>641</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="B11" s="6">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>643</v>
+      </c>
+      <c r="B12" s="7">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>644</v>
+      </c>
+      <c r="B13">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>645</v>
+      </c>
+      <c r="B14" s="7">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>646</v>
+      </c>
+      <c r="B15" s="7">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>647</v>
+      </c>
+      <c r="B16" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>648</v>
+      </c>
+      <c r="B17" s="7">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>649</v>
+      </c>
+      <c r="B18" s="6">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>650</v>
+      </c>
+      <c r="B19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>651</v>
+      </c>
+      <c r="B20" s="7">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>652</v>
+      </c>
+      <c r="B21" s="7">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>653</v>
+      </c>
+      <c r="B22" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>654</v>
+      </c>
+      <c r="B23">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>655</v>
+      </c>
+      <c r="B24" s="7">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>656</v>
+      </c>
+      <c r="B25" s="7">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>657</v>
+      </c>
+      <c r="B26" s="7">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>658</v>
+      </c>
+      <c r="B27">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>659</v>
+      </c>
+      <c r="B28">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>660</v>
+      </c>
+      <c r="B29">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>661</v>
+      </c>
+      <c r="B30" s="6">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>662</v>
+      </c>
+      <c r="B31" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>663</v>
+      </c>
+      <c r="B32" s="6">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>664</v>
+      </c>
+      <c r="B33">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>665</v>
+      </c>
+      <c r="B34">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>666</v>
+      </c>
+      <c r="B35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>667</v>
+      </c>
+      <c r="B36" s="5">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>668</v>
+      </c>
+      <c r="B37">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>669</v>
+      </c>
+      <c r="B38" s="5">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>670</v>
+      </c>
+      <c r="B39" s="5">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>671</v>
+      </c>
+      <c r="B40">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>672</v>
+      </c>
+      <c r="B41">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>673</v>
+      </c>
+      <c r="B42">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>674</v>
+      </c>
+      <c r="B43">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>675</v>
+      </c>
+      <c r="B44">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>676</v>
+      </c>
+      <c r="B45">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>677</v>
+      </c>
+      <c r="B46" s="7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>678</v>
+      </c>
+      <c r="B47">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>679</v>
+      </c>
+      <c r="B48">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>680</v>
+      </c>
+      <c r="B49" s="5">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>681</v>
+      </c>
+      <c r="B50">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>682</v>
+      </c>
+      <c r="B51" s="5">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>683</v>
+      </c>
+      <c r="B52">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>684</v>
+      </c>
+      <c r="B53">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>685</v>
+      </c>
+      <c r="B54" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>686</v>
+      </c>
+      <c r="B55">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>687</v>
+      </c>
+      <c r="B56">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>688</v>
+      </c>
+      <c r="B57" s="5">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>689</v>
+      </c>
+      <c r="B58" s="5">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>690</v>
+      </c>
+      <c r="B59">
+        <v>344</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$E$3=$F$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B32 B61">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$F4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:B59">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$F33=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixes missing geometries and projections
</commit_message>
<xml_diff>
--- a/para_comparar.xlsx
+++ b/para_comparar.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/desiertos/side/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{58FFB29D-156C-6F4B-BE3D-6B8837C6580F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6AD942-D610-B448-8335-6DC9E79E5C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="960" windowWidth="24540" windowHeight="13680" activeTab="3"/>
+    <workbookView xWindow="720" yWindow="960" windowWidth="24540" windowHeight="13680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="para_comparar_dept" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="para_comparar_dept" type="6" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="para_comparar_dept" type="6" refreshedVersion="7" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="/Users/tiago/Documents/github/desiertos/side/para_comparar_dept.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="3">
         <textField type="skip"/>
@@ -48,7 +48,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="para_comparar_mun" type="6" refreshedVersion="7" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="para_comparar_mun" type="6" refreshedVersion="7" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="/Users/tiago/Documents/github/desiertos/side/para_comparar_mun.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="13">
         <textField type="skip"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="690">
   <si>
     <t>nam</t>
   </si>
@@ -1874,9 +1874,6 @@
   </si>
   <si>
     <t>4607.00</t>
-  </si>
-  <si>
-    <t>Santiago del Estero</t>
   </si>
   <si>
     <t>tava como santiago</t>
@@ -2149,7 +2146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2813,11 +2810,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="para_comparar_dept_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="para_comparar_dept_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="para_comparar_mun" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="para_comparar_mun" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3116,7 +3113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B530"/>
   <sheetViews>
     <sheetView topLeftCell="A258" workbookViewId="0">
@@ -7378,7 +7375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
@@ -7522,7 +7519,7 @@
         <v>76</v>
       </c>
       <c r="I5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -7551,7 +7548,7 @@
         <v>215</v>
       </c>
       <c r="I6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -7580,7 +7577,7 @@
         <v>210</v>
       </c>
       <c r="I7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -7609,7 +7606,7 @@
         <v>228</v>
       </c>
       <c r="I8" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -7638,7 +7635,7 @@
         <v>203</v>
       </c>
       <c r="I9" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -7667,7 +7664,7 @@
         <v>75</v>
       </c>
       <c r="I10" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -7696,7 +7693,7 @@
         <v/>
       </c>
       <c r="I11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -7723,7 +7720,7 @@
         <v/>
       </c>
       <c r="I12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -8407,7 +8404,7 @@
         <v>villa_general_mitre_ciudad_autonoma_de_buenos_aires</v>
       </c>
       <c r="E41" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F41">
         <f>COUNTIF(para_comparar_dept!$A$2:$A$530,A41)</f>
@@ -8470,7 +8467,7 @@
         <v/>
       </c>
       <c r="I43" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -8499,7 +8496,7 @@
         <v/>
       </c>
       <c r="I44" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -8797,7 +8794,7 @@
         <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C57" t="s">
         <v>466</v>
@@ -8824,7 +8821,7 @@
         <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C58" t="s">
         <v>466</v>
@@ -8851,7 +8848,7 @@
         <v>276</v>
       </c>
       <c r="B59" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C59" t="s">
         <v>466</v>
@@ -8878,7 +8875,7 @@
         <v>156</v>
       </c>
       <c r="B60" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C60" t="s">
         <v>466</v>
@@ -8904,7 +8901,7 @@
         <v>164</v>
       </c>
       <c r="B61" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C61" t="s">
         <v>466</v>
@@ -8931,7 +8928,7 @@
         <v>141</v>
       </c>
       <c r="B62" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C62" t="s">
         <v>466</v>
@@ -8957,7 +8954,7 @@
         <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C63" t="s">
         <v>466</v>
@@ -8983,7 +8980,7 @@
         <v>45</v>
       </c>
       <c r="B64" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C64" t="s">
         <v>466</v>
@@ -9010,7 +9007,7 @@
         <v>149</v>
       </c>
       <c r="B65" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C65" t="s">
         <v>466</v>
@@ -9037,7 +9034,7 @@
         <v>231</v>
       </c>
       <c r="B66" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C66" t="s">
         <v>466</v>
@@ -9064,7 +9061,7 @@
         <v>38</v>
       </c>
       <c r="B67" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C67" t="s">
         <v>466</v>
@@ -9091,7 +9088,7 @@
         <v>366</v>
       </c>
       <c r="B68" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C68" t="s">
         <v>466</v>
@@ -9118,7 +9115,7 @@
         <v>430</v>
       </c>
       <c r="B69" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C69" t="s">
         <v>466</v>
@@ -9145,7 +9142,7 @@
         <v>589</v>
       </c>
       <c r="B70" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C70" t="s">
         <v>466</v>
@@ -9171,7 +9168,7 @@
         <v>175</v>
       </c>
       <c r="B71" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C71" t="s">
         <v>466</v>
@@ -9198,7 +9195,7 @@
         <v>275</v>
       </c>
       <c r="B72" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C72" t="s">
         <v>466</v>
@@ -9225,7 +9222,7 @@
         <v>24</v>
       </c>
       <c r="B73" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C73" t="s">
         <v>466</v>
@@ -9251,7 +9248,7 @@
         <v>44</v>
       </c>
       <c r="B74" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C74" t="s">
         <v>466</v>
@@ -9278,7 +9275,7 @@
         <v>91</v>
       </c>
       <c r="B75" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C75" t="s">
         <v>466</v>
@@ -9304,7 +9301,7 @@
         <v>134</v>
       </c>
       <c r="B76" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C76" t="s">
         <v>466</v>
@@ -9331,7 +9328,7 @@
         <v>367</v>
       </c>
       <c r="B77" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C77" t="s">
         <v>466</v>
@@ -9358,7 +9355,7 @@
         <v>43</v>
       </c>
       <c r="B78" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C78" t="s">
         <v>466</v>
@@ -9384,7 +9381,7 @@
         <v>173</v>
       </c>
       <c r="B79" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C79" t="s">
         <v>466</v>
@@ -9411,7 +9408,7 @@
         <v>238</v>
       </c>
       <c r="B80" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C80" t="s">
         <v>466</v>
@@ -9438,7 +9435,7 @@
         <v>355</v>
       </c>
       <c r="B81" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C81" t="s">
         <v>466</v>
@@ -9464,7 +9461,7 @@
         <v>98</v>
       </c>
       <c r="B82" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C82" t="s">
         <v>466</v>
@@ -9490,7 +9487,7 @@
         <v>372</v>
       </c>
       <c r="B83" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C83" t="s">
         <v>466</v>
@@ -9548,11 +9545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9613,10 +9610,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -9642,10 +9639,10 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -9671,10 +9668,10 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -9700,10 +9697,10 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -9729,10 +9726,10 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -9758,10 +9755,10 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -9787,10 +9784,10 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I8" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -9816,10 +9813,10 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -9845,10 +9842,10 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -9868,10 +9865,10 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -9897,10 +9894,10 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I12" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -9920,10 +9917,10 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I13" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -9949,10 +9946,10 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I14" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -9978,10 +9975,10 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I15" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -10007,10 +10004,10 @@
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I16" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -10030,10 +10027,10 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I17" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -10059,10 +10056,10 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I18" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -10088,10 +10085,10 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -10111,10 +10108,10 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I20" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -10140,10 +10137,10 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I21" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -10169,10 +10166,10 @@
         <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I22" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -10198,10 +10195,10 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I23" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -10227,10 +10224,10 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I24" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -10250,10 +10247,10 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -10273,10 +10270,10 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I26" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -10302,10 +10299,10 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I27" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -10325,10 +10322,10 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>601</v>
+        <v>466</v>
       </c>
       <c r="I28" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -10337,10 +10334,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
@@ -10360,7 +10357,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B2" s="5">
         <v>472</v>
@@ -10368,7 +10365,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B3" s="7">
         <v>158</v>
@@ -10376,7 +10373,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B4">
         <v>471</v>
@@ -10384,7 +10381,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B5">
         <v>76</v>
@@ -10392,7 +10389,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B6">
         <v>215</v>
@@ -10400,7 +10397,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B7">
         <v>210</v>
@@ -10408,7 +10405,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B8">
         <v>228</v>
@@ -10416,7 +10413,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B9">
         <v>203</v>
@@ -10424,7 +10421,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B10">
         <v>75</v>
@@ -10432,7 +10429,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B11" s="6">
         <v>227</v>
@@ -10440,7 +10437,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B12" s="7">
         <v>426</v>
@@ -10448,7 +10445,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B13">
         <v>414</v>
@@ -10456,7 +10453,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B14" s="7">
         <v>167</v>
@@ -10464,7 +10461,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B15" s="7">
         <v>387</v>
@@ -10472,7 +10469,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B16" s="6">
         <v>500</v>
@@ -10480,7 +10477,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B17" s="7">
         <v>195</v>
@@ -10488,7 +10485,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B18" s="6">
         <v>466</v>
@@ -10496,7 +10493,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B19">
         <v>24</v>
@@ -10504,7 +10501,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B20" s="7">
         <v>386</v>
@@ -10512,7 +10509,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B21" s="7">
         <v>394</v>
@@ -10520,7 +10517,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B22" s="7">
         <v>21</v>
@@ -10528,7 +10525,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B23">
         <v>67</v>
@@ -10536,7 +10533,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B24" s="7">
         <v>268</v>
@@ -10544,7 +10541,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B25" s="7">
         <v>335</v>
@@ -10552,7 +10549,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B26" s="7">
         <v>356</v>
@@ -10560,7 +10557,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B27">
         <v>294</v>
@@ -10568,7 +10565,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B28">
         <v>358</v>
@@ -10576,7 +10573,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B29">
         <v>64</v>
@@ -10584,7 +10581,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B30" s="6">
         <v>184</v>
@@ -10592,7 +10589,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B31" s="6">
         <v>4</v>
@@ -10600,7 +10597,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B32" s="6">
         <v>348</v>
@@ -10608,7 +10605,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B33">
         <v>218</v>
@@ -10616,7 +10613,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B34">
         <v>35</v>
@@ -10624,7 +10621,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B35">
         <v>392</v>
@@ -10632,7 +10629,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B36" s="5">
         <v>338</v>
@@ -10640,7 +10637,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B37">
         <v>211</v>
@@ -10648,7 +10645,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B38" s="5">
         <v>217</v>
@@ -10656,7 +10653,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B39" s="5">
         <v>244</v>
@@ -10664,7 +10661,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B40">
         <v>40</v>
@@ -10672,7 +10669,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B41">
         <v>181</v>
@@ -10680,7 +10677,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B42">
         <v>326</v>
@@ -10688,7 +10685,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B43">
         <v>37</v>
@@ -10696,7 +10693,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B44">
         <v>220</v>
@@ -10704,7 +10701,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B45">
         <v>393</v>
@@ -10712,7 +10709,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B46" s="7">
         <v>36</v>
@@ -10720,7 +10717,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B47">
         <v>246</v>
@@ -10728,7 +10725,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B48">
         <v>391</v>
@@ -10736,7 +10733,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B49" s="5">
         <v>339</v>
@@ -10744,7 +10741,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B50">
         <v>39</v>
@@ -10752,7 +10749,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B51" s="5">
         <v>337</v>
@@ -10760,7 +10757,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B52">
         <v>154</v>
@@ -10768,7 +10765,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B53">
         <v>182</v>
@@ -10776,7 +10773,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B54" s="5">
         <v>38</v>
@@ -10784,7 +10781,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B55">
         <v>243</v>
@@ -10792,7 +10789,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B56">
         <v>336</v>
@@ -10800,7 +10797,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B57" s="5">
         <v>131</v>
@@ -10808,7 +10805,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B58" s="5">
         <v>214</v>
@@ -10816,7 +10813,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B59">
         <v>344</v>

</xml_diff>